<commit_message>
Preprocessing before Power Pivot Aggregation
</commit_message>
<xml_diff>
--- a/questions_and_analysis/employee_add_fields.xlsx
+++ b/questions_and_analysis/employee_add_fields.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dumisani Mukuchura\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dumisani Mukuchura\Desktop\Projects\Excel\CycleSilicon Inc. Employee Bike Purchase Dataset – Part 2 Advanced Pivot Tables &amp; Dashboard by Dumisani Mukuchura\questions_and_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24042" windowHeight="8627"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Add_Fields" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>

</xml_diff>